<commit_message>
Finished multi-GPU with CAE. Need to fix PCA/KMeans
</commit_message>
<xml_diff>
--- a/Code/gpu_vs_time/gpu_time_test_results.xlsx
+++ b/Code/gpu_vs_time/gpu_time_test_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ORNL_Coding\Code\gpu_vs_time\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B9F3042-5764-4F84-BB22-ED999E1FFA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{904635A4-E10E-49B4-9FE5-1172D394B74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95A58FA8-506F-4E56-B639-CDE8E5815D05}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{95A58FA8-506F-4E56-B639-CDE8E5815D05}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -610,22 +610,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.9355252801413247</c:v>
+                  <c:v>1.8904493743168918</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.79718473363411635</c:v>
+                  <c:v>0.28709755902581963</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.18414332369970707</c:v>
+                  <c:v>-0.24533350781131547</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.50971333801515861</c:v>
+                  <c:v>-0.49446374755122191</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.11371860429103069</c:v>
+                  <c:v>-0.66628606270257773</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.55820248908341275</c:v>
+                  <c:v>-0.77146361527759666</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -702,22 +702,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>2.0320336244898667</c:v>
+                  <c:v>1.7742323558554192</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-0.25911838164635415</c:v>
+                  <c:v>0.44258231091368155</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-0.55062656099853169</c:v>
+                  <c:v>-4.3699550325388928E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.36651613193400767</c:v>
+                  <c:v>-0.5566144124632908</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.42788627495551568</c:v>
+                  <c:v>-0.67049345078934375</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-0.42788627495551568</c:v>
+                  <c:v>-0.94600725319108248</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2386,22 +2386,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>148.54</c:v>
+                  <c:v>144.86000000000001</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>140.65</c:v>
+                  <c:v>78.7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>142.41999999999999</c:v>
+                  <c:v>56.73</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>141.47999999999999</c:v>
+                  <c:v>46.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>143.28</c:v>
+                  <c:v>39.36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>141.34</c:v>
+                  <c:v>35.020000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2885,22 +2885,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>789.98</c:v>
+                  <c:v>709.24</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>785.5</c:v>
+                  <c:v>680.24</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>784.93</c:v>
+                  <c:v>669.65</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>785.29</c:v>
+                  <c:v>658.48</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>785.17</c:v>
+                  <c:v>656</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>785.17</c:v>
+                  <c:v>650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6509,7 +6509,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+      <selection activeCell="G79" sqref="G79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6571,10 +6571,10 @@
         <v>2.85</v>
       </c>
       <c r="F2">
-        <v>148.54</v>
+        <v>144.86000000000001</v>
       </c>
       <c r="G2">
-        <v>789.98</v>
+        <v>709.24</v>
       </c>
       <c r="J2">
         <f>AVERAGE(B2:B7)</f>
@@ -6602,10 +6602,10 @@
         <v>0.79</v>
       </c>
       <c r="F3">
-        <v>140.65</v>
+        <v>78.7</v>
       </c>
       <c r="G3">
-        <v>785.5</v>
+        <v>680.24</v>
       </c>
       <c r="J3">
         <f>AVERAGE(C2:C7)</f>
@@ -6633,10 +6633,10 @@
         <v>0.36</v>
       </c>
       <c r="F4">
-        <v>142.41999999999999</v>
+        <v>56.73</v>
       </c>
       <c r="G4">
-        <v>784.93</v>
+        <v>669.65</v>
       </c>
       <c r="J4">
         <f>AVERAGE(D2:D7)</f>
@@ -6664,10 +6664,10 @@
         <v>0.36</v>
       </c>
       <c r="F5">
-        <v>141.47999999999999</v>
+        <v>46.45</v>
       </c>
       <c r="G5">
-        <v>785.29</v>
+        <v>658.48</v>
       </c>
       <c r="J5">
         <f>AVERAGE(E2:E7)</f>
@@ -6695,18 +6695,18 @@
         <v>0.4</v>
       </c>
       <c r="F6">
-        <v>143.28</v>
+        <v>39.36</v>
       </c>
       <c r="G6">
-        <v>785.17</v>
+        <v>656</v>
       </c>
       <c r="J6">
         <f>AVERAGE(F2:F7)</f>
-        <v>142.95166666666668</v>
+        <v>66.853333333333339</v>
       </c>
       <c r="K6">
         <f>STDEV(F2:F7)</f>
-        <v>2.8872437837263849</v>
+        <v>41.263557610398401</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -6726,18 +6726,18 @@
         <v>0.75</v>
       </c>
       <c r="F7">
-        <v>141.34</v>
+        <v>35.020000000000003</v>
       </c>
       <c r="G7">
-        <v>785.17</v>
+        <v>650</v>
       </c>
       <c r="J7">
         <f>AVERAGE(G2:G7)</f>
-        <v>786.00666666666666</v>
+        <v>670.60166666666669</v>
       </c>
       <c r="K7">
         <f>STDEV(G2:G7)</f>
-        <v>1.9553482213321376</v>
+        <v>21.777493351317244</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -6759,11 +6759,11 @@
       </c>
       <c r="F9">
         <f>(F2-J$6)/K$6</f>
-        <v>1.9355252801413247</v>
+        <v>1.8904493743168918</v>
       </c>
       <c r="G9">
         <f>(G2-J$7)/K$7</f>
-        <v>2.0320336244898667</v>
+        <v>1.7742323558554192</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -6785,11 +6785,11 @@
       </c>
       <c r="F10">
         <f t="shared" ref="F10:F14" si="3">(F3-J$6)/K$6</f>
-        <v>-0.79718473363411635</v>
+        <v>0.28709755902581963</v>
       </c>
       <c r="G10">
         <f t="shared" ref="G10:G14" si="4">(G3-J$7)/K$7</f>
-        <v>-0.25911838164635415</v>
+        <v>0.44258231091368155</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -6811,11 +6811,11 @@
       </c>
       <c r="F11">
         <f t="shared" si="3"/>
-        <v>-0.18414332369970707</v>
+        <v>-0.24533350781131547</v>
       </c>
       <c r="G11">
         <f t="shared" si="4"/>
-        <v>-0.55062656099853169</v>
+        <v>-4.3699550325388928E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -6837,11 +6837,11 @@
       </c>
       <c r="F12">
         <f t="shared" si="3"/>
-        <v>-0.50971333801515861</v>
+        <v>-0.49446374755122191</v>
       </c>
       <c r="G12">
         <f t="shared" si="4"/>
-        <v>-0.36651613193400767</v>
+        <v>-0.5566144124632908</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -6863,11 +6863,11 @@
       </c>
       <c r="F13">
         <f t="shared" si="3"/>
-        <v>0.11371860429103069</v>
+        <v>-0.66628606270257773</v>
       </c>
       <c r="G13">
         <f t="shared" si="4"/>
-        <v>-0.42788627495551568</v>
+        <v>-0.67049345078934375</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -6889,11 +6889,11 @@
       </c>
       <c r="F14">
         <f t="shared" si="3"/>
-        <v>-0.55820248908341275</v>
+        <v>-0.77146361527759666</v>
       </c>
       <c r="G14">
         <f t="shared" si="4"/>
-        <v>-0.42788627495551568</v>
+        <v>-0.94600725319108248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>